<commit_message>
ongoing testing work ... ongoing work on PkRewriterMiddleware tests
</commit_message>
<xml_diff>
--- a/test/MiddlewareTests/MiddlewareTests/PkRewriter/TestJson.xlsx
+++ b/test/MiddlewareTests/MiddlewareTests/PkRewriter/TestJson.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denmi\source\repos\EDennis.AspNetCore.Base\test\MiddlewareTests\MiddlewareTests\ScopeProperties\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denmi\source\repos\EDennis.AspNetCore.Base\test\MiddlewareTests\MiddlewareTests\PkRewriter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7420EAE7-1045-4DA6-A1AE-2E562D0513F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0109AED-4757-4F5F-85B5-68A8D33D3EB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="1823" windowWidth="17992" windowHeight="10800" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="38">
   <si>
     <t>ProjectName</t>
   </si>
@@ -63,34 +63,88 @@
     <t>B</t>
   </si>
   <si>
-    <t>Get</t>
-  </si>
-  <si>
-    <t>Headers</t>
-  </si>
-  <si>
-    <t>header*hdr1=ABC&amp;header*hdr2=DEF</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
-    <t>MockHeadersApi</t>
-  </si>
-  <si>
-    <t>MockHeadersController</t>
-  </si>
-  <si>
-    <t>header*X-User=jill&amp;header*X-Role=user</t>
-  </si>
-  <si>
-    <t>[{"Key":"Host","Value":"localhost"},{"Key":"X-User","Value":"larry@stooges.org"},{"Key":"X-Role","Value":"admin"},{"Key":"X-Role","Value":"user"}]</t>
-  </si>
-  <si>
-    <t>[{"Key":"Host","Value":"localhost"},{"Key":"hdr1","Value":"ABC"},{"Key":"hdr2","Value":"DEF"},{"Key":"X-User","Value":"moe@stooges.org"},{"Key":"X-Role","Value":"admin"},{"Key":"X-Role","Value":"user"}]</t>
-  </si>
-  <si>
-    <t>[{"Key":"Host","Value":"localhost"},{"Key":"X-User","Value":"curly@stooges.org"},{"Key":"X-Role","Value":"readonly"}]</t>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>{"id": -999005,"firstName": "Drew","lastName": "Carey"}</t>
+  </si>
+  <si>
+    <t>[{"id": -999001,"firstName": "Bob","lastName": "Barker"},{"id": -999002,"firstName": "Monty","lastName": "Hall"},{"id": -999005,"firstName": "Drew","lastName": "Carey"}]</t>
+  </si>
+  <si>
+    <t>ExpectedBypass</t>
+  </si>
+  <si>
+    <t>[{"id": -999001,"firstName": "Bob","lastName": "Barker"},{"id": -999002,"firstName": "Monty","lastName": "Hall"},{"id": -501005,"firstName": "Drew","lastName": "Carey"}]</t>
+  </si>
+  <si>
+    <t>[{"id": -999001,"firstName": "Bob","lastName": "Barker"},{"id": -999002,"firstName": "Monty","lastName": "Hall"},{"id": -502005,"firstName": "Drew","lastName": "Carey"}]</t>
+  </si>
+  <si>
+    <t>[{"id": -999001,"firstName": "Bob","lastName": "Barker"},{"id": -999002,"firstName": "Monty","lastName": "Hall"},{"id": -503005,"firstName": "Drew","lastName": "Carey"}]</t>
+  </si>
+  <si>
+    <t>PkRewriterApi</t>
+  </si>
+  <si>
+    <t>PersonController</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>{"id": -999001,"firstName": "Robert","lastName": "Barker"}</t>
+  </si>
+  <si>
+    <t>Input1</t>
+  </si>
+  <si>
+    <t>CreateUpdate</t>
+  </si>
+  <si>
+    <t>Input2</t>
+  </si>
+  <si>
+    <t>{"id": -999005,"firstName": "Andrew","lastName": "Carey"}</t>
+  </si>
+  <si>
+    <t>[{"id": -999001,"firstName": "Bob","lastName": "Barker"},{"id": -999002,"firstName": "Monty","lastName": "Hall"},{"id": -999005,"firstName": "Andrew","lastName": "Carey"}]</t>
+  </si>
+  <si>
+    <t>[{"id": -999001,"firstName": "Bob","lastName": "Barker"},{"id": -999002,"firstName": "Monty","lastName": "Hall"},{"id": -501005,"firstName": "Andrew","lastName": "Carey"}]</t>
+  </si>
+  <si>
+    <t>[{"id": -999001,"firstName": "Bob","lastName": "Barker"},{"id": -999002,"firstName": "Monty","lastName": "Hall"},{"id": -502005,"firstName": "Andrew","lastName": "Carey"}]</t>
+  </si>
+  <si>
+    <t>[{"id": -999001,"firstName": "Bob","lastName": "Barker"},{"id": -999002,"firstName": "Monty","lastName": "Hall"},{"id": -503005,"firstName": "Andrew","lastName": "Carey"}]</t>
+  </si>
+  <si>
+    <t>{"id": -999002,"firstName": "Monte","lastName": "Hall"}</t>
+  </si>
+  <si>
+    <t>{"id": -888001,"firstName": "Steve","lastName": "Rogers"}</t>
+  </si>
+  <si>
+    <t>QueryString</t>
+  </si>
+  <si>
+    <t>{"id": -999006,"firstName": "Wayne","lastName": "Brady"}</t>
+  </si>
+  <si>
+    <t>idNot=-999006</t>
+  </si>
+  <si>
+    <t>Query</t>
   </si>
 </sst>
 </file>
@@ -443,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DF70F6-41B8-4967-A575-80BF52770920}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -456,7 +510,7 @@
     <col min="3" max="3" width="13.86328125" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.59765625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.1328125" style="1"/>
-    <col min="6" max="6" width="9.3984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="42.73046875" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.1328125" style="1"/>
   </cols>
@@ -486,33 +540,33 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
@@ -521,24 +575,24 @@
         <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>16</v>
@@ -546,62 +600,914 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="G10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="1">
+        <v>-999005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="1">
+        <v>-999005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="1" t="s">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="1">
+        <v>-999005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>19</v>
+      <c r="G24" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="1">
+        <v>-999001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" s="1">
+        <v>-999002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" s="1">
+        <v>-888001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added configurable ExplicitIds creation option for PkRewriter middleware
</commit_message>
<xml_diff>
--- a/test/MiddlewareTests/MiddlewareTests/PkRewriter/TestJson.xlsx
+++ b/test/MiddlewareTests/MiddlewareTests/PkRewriter/TestJson.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denmi\source\repos\EDennis.AspNetCore.Base\test\MiddlewareTests\MiddlewareTests\PkRewriter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MitchellDenC\source\repos\EDennis.AspNetCore.Base\test\MiddlewareTests\MiddlewareTests\PkRewriter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0109AED-4757-4F5F-85B5-68A8D33D3EB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01199C98-E555-410F-B570-704D301C3245}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
+    <workbookView xWindow="2550" yWindow="1095" windowWidth="14940" windowHeight="11055" xr2:uid="{914E17DC-A849-42DE-BD5C-694BB7A8109C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="42">
   <si>
     <t>ProjectName</t>
   </si>
@@ -145,6 +145,18 @@
   </si>
   <si>
     <t>Query</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>{"firstName": "Drew","lastName": "Carey"}</t>
+  </si>
+  <si>
+    <t>[{"id": -999001,"firstName": "Bob","lastName": "Barker"},{"id": -999002,"firstName": "Monty","lastName": "Hall"},{"id": -999301,"firstName": "Drew","lastName": "Carey"}]</t>
+  </si>
+  <si>
+    <t>[{"id": -999001,"firstName": "Bob","lastName": "Barker"},{"id": -999002,"firstName": "Monty","lastName": "Hall"},{"id": -501301,"firstName": "Drew","lastName": "Carey"}]</t>
   </si>
 </sst>
 </file>
@@ -497,25 +509,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3DF70F6-41B8-4967-A575-80BF52770920}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26:D34"/>
+    <sheetView tabSelected="1" topLeftCell="E41" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.59765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.86328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.59765625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1328125" style="1"/>
-    <col min="6" max="6" width="13.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.73046875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1328125" style="1"/>
+    <col min="1" max="1" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="17.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="42.7109375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,7 +550,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -558,7 +570,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -578,7 +590,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -598,7 +610,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -618,7 +630,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -638,7 +650,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -658,7 +670,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -678,7 +690,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -698,7 +710,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -718,7 +730,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -741,7 +753,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -764,7 +776,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -787,7 +799,7 @@
         <v>-999005</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -810,7 +822,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -833,7 +845,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -856,7 +868,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
@@ -879,7 +891,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -902,7 +914,7 @@
         <v>-999005</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -925,7 +937,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -948,7 +960,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -971,7 +983,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -994,7 +1006,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -1017,7 +1029,7 @@
         <v>-999005</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
@@ -1040,7 +1052,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
@@ -1063,7 +1075,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
@@ -1086,7 +1098,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
@@ -1109,7 +1121,7 @@
         <v>-999001</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
@@ -1132,7 +1144,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>19</v>
       </c>
@@ -1155,7 +1167,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>19</v>
       </c>
@@ -1178,7 +1190,7 @@
         <v>-999002</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>19</v>
       </c>
@@ -1201,7 +1213,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>19</v>
       </c>
@@ -1224,7 +1236,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -1247,7 +1259,7 @@
         <v>-888001</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>19</v>
       </c>
@@ -1270,7 +1282,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>19</v>
       </c>
@@ -1290,7 +1302,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>19</v>
       </c>
@@ -1310,7 +1322,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
@@ -1330,7 +1342,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>19</v>
       </c>
@@ -1350,7 +1362,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>19</v>
       </c>
@@ -1370,7 +1382,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>19</v>
       </c>
@@ -1390,7 +1402,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>19</v>
       </c>
@@ -1410,7 +1422,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>19</v>
       </c>
@@ -1430,7 +1442,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>19</v>
       </c>
@@ -1450,7 +1462,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>19</v>
       </c>
@@ -1470,7 +1482,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>19</v>
       </c>
@@ -1490,7 +1502,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>19</v>
       </c>
@@ -1508,6 +1520,66 @@
       </c>
       <c r="G46" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>